<commit_message>
Novas opções de controle
Tutorial atualizado
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moothz\Documents\GitHub\sipt-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63966B1-0EF8-4590-960D-0AFB2383AA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB849A76-21B9-4F58-B12C-6FD7E628F9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{2DDB9AE4-77D6-44B3-AC90-B9B869EC2638}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{2DDB9AE4-77D6-44B3-AC90-B9B869EC2638}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
   <si>
     <t>Ano</t>
   </si>
@@ -144,28 +144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -211,7 +190,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -539,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9178D6BA-827C-4CA8-A8D4-773DE9432587}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,45 +604,196 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1">
-    <cfRule type="duplicateValues" dxfId="11" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1">
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="NÃO">
-      <formula>NOT(ISERROR(SEARCH("NÃO",M1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="SIM">
-      <formula>NOT(ISERROR(SEARCH("SIM",M1)))</formula>
-    </cfRule>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="duplicateValues" dxfId="8" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:N1">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="SIM">
-      <formula>NOT(ISERROR(SEARCH("SIM",J1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
     <cfRule type="duplicateValues" dxfId="5" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1">
-    <cfRule type="duplicateValues" dxfId="4" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="21"/>
+  <conditionalFormatting sqref="J1:N1">
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="SIM">
+      <formula>NOT(ISERROR(SEARCH("SIM",J1)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="duplicateValues" dxfId="2" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1">
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="NÃO">
-      <formula>NOT(ISERROR(SEARCH("NÃO",N1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="SIM">
-      <formula>NOT(ISERROR(SEARCH("SIM",N1)))</formula>
+  <conditionalFormatting sqref="M1:N1">
+    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="NÃO">
+      <formula>NOT(ISERROR(SEARCH("NÃO",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>